<commit_message>
02: Plasma potencial plots, exported graphs
</commit_message>
<xml_diff>
--- a/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
+++ b/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB63E8F-2733-400E-953F-26BEA69719A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -78,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,7 +126,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -121,12 +134,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -168,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,9 +217,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,6 +269,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -411,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C12" sqref="C8:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -581,7 +631,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
02: Export rest of the graphs, protocol progress
</commit_message>
<xml_diff>
--- a/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
+++ b/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB63E8F-2733-400E-953F-26BEA69719A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D366DB9-3B70-472E-8128-B8A69BD2D9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,6 +92,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,9 +124,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -465,7 +469,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C8:C12"/>
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +491,7 @@
         <f>0.0001</f>
         <v>1E-4</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="2">
         <f>PI()*I1*H1</f>
         <v>2.5132741228718346E-6</v>
       </c>

</xml_diff>

<commit_message>
02: Correct, to do: T_e, derivations
</commit_message>
<xml_diff>
--- a/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
+++ b/02_JednoduchaSonda/data/JednoduchaSonda.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D366DB9-3B70-472E-8128-B8A69BD2D9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7667D60A-8FFB-46F9-9C68-AFDFBE3AD41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="3120" windowWidth="28800" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>vztahujeme sondu k anodě</t>
   </si>
@@ -52,9 +52,6 @@
     <t>v datech</t>
   </si>
   <si>
-    <t>čas</t>
-  </si>
-  <si>
     <t>hodnoty (index) rozhasené, zesynchonizovat časem</t>
   </si>
   <si>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>v [m2]</t>
+  </si>
+  <si>
+    <t>p pro Pirani</t>
+  </si>
+  <si>
+    <t>zaokrouhlení</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1">
         <v>8.0000000000000002E-3</v>
@@ -496,10 +499,10 @@
         <v>2.5132741228718346E-6</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -522,11 +525,14 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -539,10 +545,17 @@
       <c r="D5">
         <v>40</v>
       </c>
+      <c r="F5">
+        <f>C5*1.59</f>
+        <v>159</v>
+      </c>
+      <c r="G5">
+        <v>160</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -550,10 +563,17 @@
       <c r="D6">
         <v>30</v>
       </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F12" si="0">C6*1.59</f>
+        <v>159</v>
+      </c>
+      <c r="G6">
+        <v>160</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -561,10 +581,17 @@
       <c r="D7">
         <v>50</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="G7">
+        <v>160</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>200</v>
@@ -572,10 +599,17 @@
       <c r="D8">
         <v>40</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+      <c r="G8">
+        <v>320</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -583,10 +617,17 @@
       <c r="D9">
         <v>40</v>
       </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>79.5</v>
+      </c>
+      <c r="G9">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -594,10 +635,17 @@
       <c r="D10">
         <v>40</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>31.8</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -605,16 +653,30 @@
       <c r="D11">
         <v>40</v>
       </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>15.9</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12">
         <v>40</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>7.95</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>